<commit_message>
A few new zip to DD mappings.
</commit_message>
<xml_diff>
--- a/data/Zip_to_DD_Site.xlsx
+++ b/data/Zip_to_DD_Site.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\fnsb-benchmark\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{55F89B70-109D-42A1-B7D1-FD99BD131429}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2BF4F2E9-4BFD-4C4C-9D5F-BDD3BDF23257}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_alaska_zipcode_to_station_l" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="66">
   <si>
     <t>zip_code</t>
   </si>
@@ -215,12 +215,15 @@
   </si>
   <si>
     <t>NOTE:  The Header row for the data must start on Row 5 of this spreadsheet.</t>
+  </si>
+  <si>
+    <t>KDEW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1083,11 +1086,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B275"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B283"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,263 +1124,263 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>99553</v>
+        <v>99109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>99571</v>
+        <v>99501</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>99583</v>
+        <v>99502</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>99612</v>
+        <v>99503</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>99661</v>
+        <v>99504</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>99546</v>
+        <v>99505</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>99547</v>
+        <v>99506</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>99591</v>
+        <v>99507</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>99638</v>
+        <v>99508</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>99660</v>
+        <v>99509</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>99685</v>
+        <v>99510</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>99692</v>
+        <v>99511</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>99545</v>
+        <v>99513</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>99551</v>
+        <v>99514</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>99552</v>
+        <v>99515</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>99557</v>
+        <v>99516</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>99559</v>
+        <v>99517</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>99561</v>
+        <v>99518</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>99575</v>
+        <v>99519</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>99578</v>
+        <v>99520</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>99589</v>
+        <v>99521</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>99607</v>
+        <v>99522</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>99609</v>
+        <v>99523</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>99614</v>
+        <v>99524</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>99621</v>
+        <v>99529</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>99622</v>
+        <v>99530</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>99626</v>
+        <v>99545</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>99630</v>
+        <v>99546</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>99634</v>
+        <v>99547</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>99637</v>
+        <v>99548</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>99641</v>
+        <v>99549</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>99651</v>
+        <v>99550</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>99655</v>
+        <v>99551</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>6</v>
@@ -1385,122 +1388,122 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>99656</v>
+        <v>99552</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>99668</v>
+        <v>99553</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>99679</v>
+        <v>99554</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>99680</v>
+        <v>99555</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>99681</v>
+        <v>99556</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>99690</v>
+        <v>99557</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>99613</v>
+        <v>99558</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>99633</v>
+        <v>99559</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>99670</v>
+        <v>99561</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>99704</v>
+        <v>99563</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>99729</v>
+        <v>99564</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>99743</v>
+        <v>99565</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>99744</v>
+        <v>99566</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>99755</v>
+        <v>99567</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>99555</v>
+        <v>99568</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1513,231 +1516,231 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>99576</v>
+        <v>99571</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>99580</v>
+        <v>99572</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>99628</v>
+        <v>99573</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>99636</v>
+        <v>99574</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>99678</v>
+        <v>99575</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>99827</v>
+        <v>99576</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>99801</v>
+        <v>99577</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>99802</v>
+        <v>99578</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>99803</v>
+        <v>99579</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>99811</v>
+        <v>99580</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>99812</v>
+        <v>99581</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>99821</v>
+        <v>99583</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>99824</v>
+        <v>99585</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>99850</v>
+        <v>99586</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>99556</v>
+        <v>99587</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>99568</v>
+        <v>99588</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>99572</v>
+        <v>99589</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>99603</v>
+        <v>99590</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>99605</v>
+        <v>99591</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>99610</v>
+        <v>99599</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>99611</v>
+        <v>99602</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>99631</v>
+        <v>99603</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>99635</v>
+        <v>99604</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>99639</v>
+        <v>99605</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>99663</v>
+        <v>99606</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>99664</v>
+        <v>99607</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>99669</v>
+        <v>99608</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>99672</v>
+        <v>99609</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>99682</v>
+        <v>99610</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>17</v>
@@ -1745,39 +1748,39 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>99901</v>
+        <v>99611</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>99928</v>
+        <v>99612</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>99950</v>
+        <v>99613</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>99550</v>
+        <v>99614</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>99608</v>
+        <v>99615</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>22</v>
@@ -1785,7 +1788,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>99615</v>
+        <v>99619</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>22</v>
@@ -1793,31 +1796,31 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>99619</v>
+        <v>99620</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>99624</v>
+        <v>99621</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>99643</v>
+        <v>99622</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>99644</v>
+        <v>99624</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>22</v>
@@ -1825,175 +1828,175 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>99697</v>
+        <v>99625</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>99548</v>
+        <v>99626</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>99549</v>
+        <v>99627</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>99564</v>
+        <v>99628</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>99565</v>
+        <v>99629</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>99579</v>
+        <v>99629</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>99606</v>
+        <v>99630</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>99625</v>
+        <v>99631</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>99640</v>
+        <v>99632</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>99647</v>
+        <v>99633</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>99648</v>
+        <v>99634</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>99649</v>
+        <v>99635</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>99653</v>
+        <v>99636</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>99629</v>
+        <v>99637</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>99645</v>
+        <v>99638</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>99652</v>
+        <v>99639</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>99654</v>
+        <v>99640</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>99667</v>
+        <v>99641</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>99674</v>
+        <v>99643</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>99676</v>
+        <v>99644</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>99683</v>
+        <v>99645</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>99687</v>
+        <v>99645</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>25</v>
@@ -2001,31 +2004,31 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>99688</v>
+        <v>99647</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>99694</v>
+        <v>99648</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>99659</v>
+        <v>99649</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>99671</v>
+        <v>99650</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>28</v>
@@ -2033,775 +2036,775 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>99684</v>
+        <v>99651</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>99739</v>
+        <v>99652</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>99742</v>
+        <v>99652</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>99753</v>
+        <v>99653</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>99762</v>
+        <v>99654</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>99769</v>
+        <v>99654</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>99771</v>
+        <v>99655</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>99772</v>
+        <v>99656</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>99778</v>
+        <v>99657</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>99784</v>
+        <v>99658</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>99785</v>
+        <v>99659</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>99721</v>
+        <v>99660</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>99723</v>
+        <v>99661</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>99734</v>
+        <v>99662</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>99747</v>
+        <v>99663</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>99759</v>
+        <v>99664</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>99766</v>
+        <v>99665</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>99782</v>
+        <v>99666</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>99789</v>
+        <v>99667</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>99791</v>
+        <v>99667</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>99727</v>
+        <v>99668</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>99736</v>
+        <v>99669</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>99749</v>
+        <v>99670</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>99750</v>
+        <v>99671</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>99751</v>
+        <v>99672</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>99752</v>
+        <v>99674</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>99761</v>
+        <v>99674</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>99763</v>
+        <v>99675</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>99770</v>
+        <v>99676</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>99773</v>
+        <v>99676</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>99786</v>
+        <v>99677</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>99903</v>
+        <v>99678</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>99918</v>
+        <v>99679</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>99919</v>
+        <v>99680</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>99921</v>
+        <v>99681</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>99922</v>
+        <v>99682</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>99923</v>
+        <v>99683</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>99925</v>
+        <v>99683</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>99926</v>
+        <v>99684</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>99927</v>
+        <v>99685</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>99835</v>
+        <v>99686</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>99820</v>
+        <v>99687</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>99825</v>
+        <v>99687</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>99826</v>
+        <v>99688</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>99829</v>
+        <v>99688</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>99832</v>
+        <v>99689</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>99840</v>
+        <v>99690</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>99841</v>
+        <v>99691</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>99731</v>
+        <v>99692</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>99732</v>
+        <v>99693</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>99737</v>
+        <v>99694</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>99738</v>
+        <v>99694</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>99764</v>
+        <v>99695</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>99776</v>
+        <v>99697</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>99780</v>
+        <v>99701</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>99566</v>
+        <v>99702</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>99573</v>
+        <v>99703</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>99574</v>
+        <v>99704</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>99586</v>
+        <v>99705</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>99588</v>
+        <v>99706</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>99677</v>
+        <v>99707</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>99686</v>
+        <v>99709</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>99693</v>
+        <v>99712</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>99554</v>
+        <v>99714</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>99563</v>
+        <v>99720</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>99581</v>
+        <v>99721</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>99585</v>
+        <v>99722</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>99604</v>
+        <v>99723</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>99620</v>
+        <v>99724</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>99632</v>
+        <v>99725</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>99650</v>
+        <v>99726</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>99657</v>
+        <v>99727</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>99658</v>
+        <v>99729</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>99662</v>
+        <v>99730</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>99666</v>
+        <v>99731</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>99830</v>
+        <v>99732</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>99833</v>
+        <v>99733</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>99836</v>
+        <v>99734</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>99929</v>
+        <v>99736</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>99689</v>
+        <v>99737</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>99558</v>
+        <v>99738</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>99590</v>
+        <v>99739</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>99602</v>
+        <v>99740</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>99627</v>
+        <v>99741</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>99665</v>
+        <v>99742</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>99675</v>
+        <v>99743</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>99691</v>
+        <v>99744</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>99720</v>
+        <v>99745</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>99722</v>
+        <v>99746</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>99724</v>
+        <v>99747</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>99726</v>
+        <v>99748</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>99730</v>
+        <v>99749</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>99733</v>
+        <v>99750</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>99740</v>
+        <v>99751</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>99741</v>
+        <v>99752</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>99745</v>
+        <v>99753</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>99746</v>
+        <v>99754</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>29</v>
@@ -2809,23 +2812,23 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>99748</v>
+        <v>99755</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>99754</v>
+        <v>99756</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>99756</v>
+        <v>99757</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>56</v>
@@ -2833,18 +2836,18 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>99757</v>
+        <v>99758</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>99758</v>
+        <v>99759</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -2857,111 +2860,111 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>99765</v>
+        <v>99761</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>99767</v>
+        <v>99762</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>99768</v>
+        <v>99763</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>99774</v>
+        <v>99764</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>99777</v>
+        <v>99765</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>99781</v>
+        <v>99766</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>99788</v>
+        <v>99767</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
-        <v>99705</v>
+        <v>99768</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>99709</v>
+        <v>99769</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>99775</v>
+        <v>99770</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>99702</v>
+        <v>99771</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>99703</v>
+        <v>99772</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>99706</v>
+        <v>99773</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>99701</v>
+        <v>99774</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>58</v>
@@ -2969,7 +2972,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>99790</v>
+        <v>99775</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>58</v>
@@ -2977,309 +2980,376 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>99714</v>
+        <v>99776</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>99712</v>
+        <v>99777</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>99510</v>
+        <v>99778</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>99511</v>
+        <v>99780</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
-        <v>99513</v>
+        <v>99781</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
-        <v>99514</v>
+        <v>99782</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
-        <v>99515</v>
+        <v>99784</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
-        <v>99521</v>
+        <v>99785</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
-        <v>99522</v>
+        <v>99786</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>99523</v>
+        <v>99788</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>99524</v>
+        <v>99789</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>99529</v>
+        <v>99790</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>99501</v>
+        <v>99791</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>99502</v>
+        <v>99801</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
-        <v>99503</v>
+        <v>99802</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
-        <v>99504</v>
+        <v>99803</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
-        <v>99507</v>
+        <v>99811</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
-        <v>99508</v>
+        <v>99812</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
-        <v>99509</v>
+        <v>99820</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
-        <v>99516</v>
+        <v>99821</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>99517</v>
+        <v>99824</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>99518</v>
+        <v>99825</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>99519</v>
+        <v>99826</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>99520</v>
+        <v>99827</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>99530</v>
+        <v>99829</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
-        <v>99599</v>
+        <v>99830</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>99695</v>
+        <v>99832</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>99629</v>
+        <v>99833</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
-        <v>99645</v>
+        <v>99835</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
-        <v>99652</v>
+        <v>99836</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>99654</v>
+        <v>99840</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>99667</v>
+        <v>99841</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
-        <v>99674</v>
+        <v>99850</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
-        <v>99676</v>
+        <v>99901</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
-        <v>99683</v>
+        <v>99903</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
-        <v>99687</v>
+        <v>99918</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
-        <v>99688</v>
+        <v>99919</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
-        <v>99694</v>
+        <v>99921</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="1">
+        <v>99922</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>99923</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>99925</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>99926</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
+        <v>99927</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
+        <v>99928</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>99929</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>99950</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A6:B283">
+    <sortCondition ref="A6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>